<commit_message>
update ideal neighborhood data
Signed-off-by: Gilang Pamungkas <gilang.pamungkas.25@ucl.ac.uk>
</commit_message>
<xml_diff>
--- a/Web/data/ideal_neighborhood.xlsx
+++ b/Web/data/ideal_neighborhood.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilangpamungkas/Documents/MSc Connected Environments/CASA 0017 Web Architecture/Housing Markets Across London/Web/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CABCC4-673E-7846-8883-BA0AC8EA3B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7931478A-4364-894E-8B9D-A39287EEA8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17260" xr2:uid="{EB91D25A-82E6-5343-923F-B3D3A6A42EA1}"/>
   </bookViews>
@@ -867,7 +867,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>